<commit_message>
Aula 5 excel planning files added
</commit_message>
<xml_diff>
--- a/Aula_Pratica_05/Preparação do 2.1.xlsx
+++ b/Aula_Pratica_05/Preparação do 2.1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Linguagem Simbólica</t>
   </si>
@@ -63,9 +63,6 @@
     <t>000</t>
   </si>
   <si>
-    <t>JNZ(1)</t>
-  </si>
-  <si>
     <t>R1 ← A</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
   </si>
   <si>
     <t>01</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>A + X</t>
@@ -118,9 +112,6 @@
   </si>
   <si>
     <t>15 (F)</t>
-  </si>
-  <si>
-    <t>FIM</t>
   </si>
 </sst>
 </file>
@@ -164,7 +155,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +186,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -208,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -217,12 +214,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -238,9 +229,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -253,26 +241,7 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -282,6 +251,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -567,7 +573,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1"/>
@@ -577,356 +583,334 @@
     <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="7.88671875" customWidth="1"/>
-    <col min="9" max="10" width="7.77734375" style="8" customWidth="1"/>
+    <col min="9" max="10" width="7.77734375" style="6" customWidth="1"/>
     <col min="11" max="24" width="7.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="19" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="20"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>24</v>
+      <c r="A3" s="15" t="s">
+        <v>22</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>31</v>
+      <c r="D3" s="16" t="s">
+        <v>16</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="7" t="str">
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="4" t="str">
         <f t="shared" ref="I3:I8" si="0">BIN2HEX(CONCATENATE(B3,C3,D3))</f>
         <v>50</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="4">
         <f t="shared" ref="J3:J8" si="1">BIN2DEC(CONCATENATE(B3,C3,D3))</f>
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>23</v>
+      <c r="A4" s="15" t="s">
+        <v>21</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>31</v>
+      <c r="C4" s="16" t="s">
+        <v>29</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="7" t="str">
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="4">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>28</v>
+      <c r="A5" s="15" t="s">
+        <v>26</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
+      <c r="B5" s="16" t="s">
+        <v>15</v>
       </c>
-      <c r="C5" s="28" t="s">
-        <v>18</v>
+      <c r="C5" s="24" t="s">
+        <v>17</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="7" t="str">
+      <c r="D5" s="24"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>A0</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="4">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
+      <c r="A6" s="15" t="s">
+        <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="F6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="7" t="str">
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
+      <c r="A7" s="15" t="s">
+        <v>23</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5" t="s">
+      <c r="F7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="7" t="str">
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="4">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>26</v>
+      <c r="A8" s="15" t="s">
+        <v>24</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>16</v>
+      <c r="B8" s="16" t="s">
+        <v>15</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>27</v>
+      <c r="C8" s="24" t="s">
+        <v>25</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="30" t="s">
-        <v>33</v>
-      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
-      <c r="I8" s="7" t="str">
+      <c r="I8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>A5</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="4">
         <f t="shared" si="1"/>
         <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A18" s="12"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>

</xml_diff>